<commit_message>
Actualización Carpeta Negociación 24/03/2022
Docs: Se agrego información adicional a los documentos
</commit_message>
<xml_diff>
--- a/Negociacion/FICHAS TECNICAS DEL PROYECTO (1).xlsx
+++ b/Negociacion/FICHAS TECNICAS DEL PROYECTO (1).xlsx
@@ -13,21 +13,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
   <si>
-    <t xml:space="preserve">FICHA TÉCNICA DE HARDWARE </t>
+    <t>FICHA TÉCNICA DE HARDWARE</t>
   </si>
   <si>
-    <t xml:space="preserve">NOMBRE DEL DISPOSITIVO </t>
+    <t>NOMBRE DEL DISPOSITIVO</t>
   </si>
   <si>
     <t>Computador Todo en Uno (Para aplicaciones de uso general)</t>
   </si>
   <si>
-    <t xml:space="preserve">SOLUCION-PROYECTO </t>
+    <t>SOLUCIÓN PROYECTO</t>
   </si>
   <si>
-    <t xml:space="preserve">Solución informatica para proyecto de gestion del proceso de contratación en obras civiles </t>
+    <t>Solución informática para proyecto de gestión del proceso de contratación en obras civiles</t>
   </si>
   <si>
     <t>ESPECIFICACIONES MÍNIMAS REQUERIDAS</t>
@@ -36,7 +36,7 @@
     <t>Las características mínimas obligatorias para cada uno de los dispositivos son:</t>
   </si>
   <si>
-    <t xml:space="preserve">CARACTERISTICAS FISICAS </t>
+    <t>CARACTERÍSTICAS FÍSICAS</t>
   </si>
   <si>
     <t>ITEM</t>
@@ -45,19 +45,19 @@
     <t>CANTIDAD</t>
   </si>
   <si>
-    <t xml:space="preserve">COMPONENTE </t>
+    <t>COMPONENTE</t>
   </si>
   <si>
     <t>Monitor De 23.8" FHD (1920x1080), WVA, retroiluminación LED, sin bordes, 250 nits, Opcional: Táctil</t>
   </si>
   <si>
-    <t xml:space="preserve">Mouse inalambrico, óptico de dos botones </t>
+    <t>Mouse inalambrico, óptico de dos botones</t>
   </si>
   <si>
     <t>Tamaño completo Latin American Spanish</t>
   </si>
   <si>
-    <t>altavoces Incorporados  3W</t>
+    <t>altavoces Incorporados 3W</t>
   </si>
   <si>
     <t>Camara de 720 mpx</t>
@@ -69,10 +69,7 @@
     <t>Manuales del Equipo</t>
   </si>
   <si>
-    <t>ESPECIFICACIONES TECNICAS</t>
-  </si>
-  <si>
-    <t>COMPONENTE</t>
+    <t>ESPECIFICACIONES TÉCNICAS</t>
   </si>
   <si>
     <t>Procesador: Intel Core i3-10100T Processor ( 3.00GHz 6MB )</t>
@@ -81,16 +78,16 @@
     <t>Sistema Operativo: Windows 10 Home Single Language 64</t>
   </si>
   <si>
-    <t>Memoria:  8.0GB DDR4-3200 SDRAM SODIMM 3200MHz (2 x 4.0GB)</t>
+    <t>Memoria: 8.0GB DDR4-3200 SDRAM SODIMM 3200MHz (2 x 4.0GB)</t>
   </si>
   <si>
     <t>Almacenamiento: 1TB 5400 rpm+128GB SSD PCIe</t>
   </si>
   <si>
-    <t>Conexion Inalambrica: Intel Wi-Fi 6 22260 2x2+BT5.0 no vPro</t>
+    <t>Conexión Inalámbrica: Intel Wi-Fi 6 22260 2x2+BT5.0 no vPro</t>
   </si>
   <si>
-    <t>Tarjeta Grafica: Intel UHD</t>
+    <t>Tarjeta Gráfica: Intel UHD</t>
   </si>
   <si>
     <t>Conectividad: 802.11ax wireless, Wi-Fi + Bluetooth 5.0 combo adapter, 2x2, M.2 card</t>
@@ -99,22 +96,22 @@
     <t>---</t>
   </si>
   <si>
-    <t>Puertos/Ranuras Atrás: 2 x USB 2.0, 1 x USB 3.1 Gen1, entrada de alimentación, Ethernet (RJ-45), HDMI-out</t>
+    <t>Puertos/Ranuras Atrás: 2 x USB 2.0, 1 x USB 3.1 Gen 1, entrada de alimentación, Ethernet (RJ-45), HDMI-out</t>
   </si>
   <si>
-    <t>Puertos/Ranuras Izquierda: 1 USB 3.1 Gen1, toma combinada de auriculares/micrófono (3.5mm), media card reade</t>
+    <t>Puertos/Ranuras Izquierda: 1 USB 3.1 Gen 1, toma combinada de auriculares/micrófono (3.5mm), media card reader</t>
   </si>
   <si>
-    <t>GARANTIA</t>
+    <t>GARANTÍA</t>
   </si>
   <si>
     <t>1 AÑO</t>
   </si>
   <si>
-    <t>El Equipo y todos sus componentes  (Depósito o Con transporte)</t>
+    <t>El Equipo y todos sus componentes (Depósito o Con transporte)</t>
   </si>
   <si>
-    <t>FICHA TÉCNICA DE HARDWARE  - USUARIO</t>
+    <t>FICHA TÉCNICA DE HARDWARE - USUARIO</t>
   </si>
   <si>
     <t>Computador All In One</t>
@@ -123,88 +120,79 @@
     <t>Las características mínimas obligatorias para el dispositivo son:</t>
   </si>
   <si>
-    <t xml:space="preserve">No tiene Unidad de CD/DVD Integrada  </t>
+    <t>No tiene Unidad de CD/DVD Integrada</t>
   </si>
   <si>
-    <t xml:space="preserve">Alámbrico Convencional </t>
+    <t>Alámbrico Convencional</t>
   </si>
   <si>
-    <t>Cámara de privacidad HP True Vision HD</t>
+    <t>Cámara de privacidad HP Truevision HD</t>
   </si>
   <si>
-    <t xml:space="preserve">Cámara WEB Integrada </t>
+    <t>Cámara WEB Integrada</t>
   </si>
   <si>
-    <t xml:space="preserve">Teclado Alámbrico, Mouse Alámbrico </t>
+    <t>Teclado Inalámbrico, Mouse Alámbrico</t>
   </si>
   <si>
-    <t xml:space="preserve">Memoria RAM: 4 GB  </t>
+    <t>Memoria RAM: 4 GB</t>
   </si>
   <si>
-    <t xml:space="preserve">Disco Duro (HDD) </t>
+    <t>Disco Duro (HDD)</t>
   </si>
   <si>
-    <t>Capacidad Disco Duro: 500  GB</t>
+    <t>Capacidad Disco Duro: 500 GB</t>
   </si>
   <si>
     <t>Marca Procesador: INTEL</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipo Procesador: Intel Pentium </t>
+    <t>Tipo Procesador: Intel Pentium</t>
   </si>
   <si>
-    <t xml:space="preserve">Modelo del Procesador: Intel Pentium J5040  </t>
+    <t>Modelo del Procesador: Intel Pentium J 5040</t>
   </si>
   <si>
-    <t xml:space="preserve">No Tiene Tarjeta Video/Grafica Independiente </t>
+    <t>No Tiene Tarjeta Video/Grafica Independiente</t>
   </si>
   <si>
-    <t xml:space="preserve">Sistema Operativo: Windows  </t>
+    <t>Sistema Operativo: Windows</t>
   </si>
   <si>
-    <t xml:space="preserve">Versión Sistema Operativo: Windows 10 Home 64 </t>
+    <t>Versión Sistema Operativo: Windows 10 Home 64</t>
   </si>
   <si>
-    <t>No. de Núcleos del Procesador: 4  Nucleos</t>
+    <t>No. de Núcleos del Procesador: 4 Nucleos</t>
   </si>
   <si>
-    <t xml:space="preserve">Velocidad del Procesador: 2 </t>
+    <t>Velocidad del Procesador: 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Resolución Pantalla: Full HD </t>
+    <t>Resolución Pantalla: Full HD</t>
   </si>
   <si>
-    <t xml:space="preserve">Tamaño Pantalla: 20.7  Pulgadas </t>
+    <t>Tamaño Pantalla: 20.7 Pulgadas</t>
   </si>
   <si>
-    <t xml:space="preserve">Opciones de Conectividad: Bluetooth, WiFi </t>
+    <t>Opciones de Conectividad: Bluetooth, WiFi</t>
   </si>
   <si>
-    <t>No. Puertos USB: 4  Puertos</t>
+    <t>No. Puertos USB: 4 Puertos</t>
   </si>
   <si>
-    <t xml:space="preserve">No. Salidas de Audio: 1  Puertos  </t>
+    <t>No. Salidas de Audio: 1 Puertos</t>
   </si>
   <si>
     <t>12 Meses</t>
   </si>
   <si>
-    <t xml:space="preserve">El Equipo y todos sus componentes  (Depósito o Con transporte) </t>
-  </si>
-  <si>
     <t>FICHA TÉCNICA - HOSTING</t>
-  </si>
-  <si>
-    <t>NOMBRE DEL DISPOSITIVO</t>
   </si>
   <si>
     <t>Click Panda - Hosting compartido, paquete avanzado</t>
   </si>
   <si>
-    <t>SOLUCIÓN PROYECTO</t>
-  </si>
-  <si>
-    <t>Solución informatica web para proyecto de gestion del proceso de contratación en obras civiles alojada en la nube.</t>
+    <t>Solución informática web para proyecto de gestión del proceso de contratación en obras civiles alojada en la nube.</t>
   </si>
   <si>
     <t>Las componentes mínimos obligatorios establecidos por click panda para un alojamiento web (hosting) con certificación de seguridad son:</t>
@@ -219,7 +207,7 @@
     <t>18 GB</t>
   </si>
   <si>
-    <t>Espacio de alamcenamiento en el disco duro</t>
+    <t>Espacio de almacenamiento en el disco duro</t>
   </si>
   <si>
     <t>500 GB</t>
@@ -240,13 +228,13 @@
     <t>Cuentas de correo</t>
   </si>
   <si>
-    <t>Insalación CMS (Content Management System)</t>
+    <t>Instalación CMS (Content Management System)</t>
   </si>
   <si>
     <t>Administrador DNS avanzado (Domain Name System)</t>
   </si>
   <si>
-    <t>Cuentas FTP (File Trsnfer Protocol)</t>
+    <t>Cuentas FTP (File Transfer Protocol)</t>
   </si>
   <si>
     <t>Bases de Datos</t>
@@ -270,7 +258,7 @@
     <t>1 TB</t>
   </si>
   <si>
-    <t>HDDx2 RAID 1</t>
+    <t>HDD x2 RAID 1</t>
   </si>
   <si>
     <t>5 TB</t>
@@ -303,14 +291,16 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
@@ -328,6 +318,7 @@
       <u/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -400,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -408,29 +399,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -439,26 +418,8 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -685,12 +646,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="4" width="16.71"/>
-    <col customWidth="1" min="5" max="5" width="16.57"/>
-    <col customWidth="1" min="8" max="8" width="22.29"/>
+    <col customWidth="1" min="3" max="3" width="14.0"/>
+    <col customWidth="1" min="4" max="4" width="14.63"/>
+    <col customWidth="1" min="5" max="5" width="14.5"/>
+    <col customWidth="1" min="8" max="8" width="19.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -732,7 +693,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3"/>
@@ -744,11 +705,11 @@
       <c r="M4" s="6"/>
     </row>
     <row r="5">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="3"/>
@@ -774,10 +735,10 @@
       <c r="M6" s="6"/>
     </row>
     <row r="7">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -792,32 +753,32 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8">
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>1.0</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>1.0</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="4"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="13"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="9"/>
     </row>
     <row r="9">
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>2.0</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>1.0</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="3"/>
@@ -825,13 +786,13 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10">
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>3.0</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>1.0</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="3"/>
@@ -839,13 +800,13 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11">
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>4.0</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>2.0</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="3"/>
@@ -853,13 +814,13 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12">
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>5.0</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>1.0</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="3"/>
@@ -867,13 +828,13 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13">
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>6.0</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>1.0</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="3"/>
@@ -881,10 +842,10 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14">
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>7.0</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="7">
         <v>1.0</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -895,7 +856,7 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15">
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="3"/>
@@ -905,141 +866,141 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16">
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17">
-      <c r="C17" s="17">
+      <c r="C17" s="7">
         <v>1.0</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="7">
         <v>1.0</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>20</v>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18">
-      <c r="C18" s="17">
+      <c r="C18" s="7">
         <v>2.0</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="7">
         <v>1.0</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>21</v>
+      <c r="E18" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19">
-      <c r="C19" s="17">
+      <c r="C19" s="7">
         <v>3.0</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="7">
         <v>1.0</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>22</v>
+      <c r="E19" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="4"/>
     </row>
     <row r="20">
-      <c r="C20" s="17">
+      <c r="C20" s="7">
         <v>4.0</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="7">
         <v>1.0</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>23</v>
+      <c r="E20" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21">
-      <c r="C21" s="17">
+      <c r="C21" s="7">
         <v>5.0</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="7">
         <v>1.0</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>24</v>
+      <c r="E21" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="19"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22">
-      <c r="C22" s="17">
+      <c r="C22" s="7">
         <v>6.0</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="7">
         <v>1.0</v>
       </c>
-      <c r="E22" s="15" t="s">
-        <v>25</v>
+      <c r="E22" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="4"/>
     </row>
     <row r="23">
-      <c r="C23" s="17">
+      <c r="C23" s="7">
         <v>7.0</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="7">
         <v>1.0</v>
       </c>
-      <c r="E23" s="18" t="s">
-        <v>26</v>
+      <c r="E23" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4"/>
     </row>
     <row r="24">
-      <c r="C24" s="17">
+      <c r="C24" s="7">
         <v>8.0</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>28</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25">
-      <c r="C25" s="17">
+      <c r="C25" s="7">
         <v>9.0</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>29</v>
+      <c r="D25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1047,7 +1008,7 @@
     </row>
     <row r="26">
       <c r="C26" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1056,28 +1017,28 @@
       <c r="H26" s="4"/>
     </row>
     <row r="27">
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28">
-      <c r="C28" s="9">
+      <c r="C28" s="7">
         <v>1.0</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -8928,17 +8889,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="16.43"/>
-    <col customWidth="1" min="6" max="6" width="16.71"/>
-    <col customWidth="1" min="7" max="7" width="17.71"/>
-    <col customWidth="1" min="8" max="8" width="18.14"/>
+    <col customWidth="1" min="5" max="5" width="14.38"/>
+    <col customWidth="1" min="6" max="6" width="14.63"/>
+    <col customWidth="1" min="7" max="7" width="15.5"/>
+    <col customWidth="1" min="8" max="8" width="15.88"/>
   </cols>
   <sheetData>
     <row r="2">
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -8952,7 +8913,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -8963,7 +8924,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3"/>
@@ -8971,12 +8932,12 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="7" t="s">
-        <v>35</v>
+      <c r="E5" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -8993,10 +8954,10 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -9007,77 +8968,77 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8">
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>1.0</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>1.0</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>36</v>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9">
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>2.0</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>1.0</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>37</v>
+      <c r="E9" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10">
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>3.0</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>1.0</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>38</v>
+      <c r="E10" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11">
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>4.0</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>1.0</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>39</v>
+      <c r="E11" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12">
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>5.0</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>1.0</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>40</v>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13">
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="3"/>
@@ -9087,238 +9048,238 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14">
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15">
-      <c r="C15" s="17">
+      <c r="C15" s="7">
         <v>1.0</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="7">
         <v>1.0</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>41</v>
+      <c r="E15" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16">
-      <c r="C16" s="17">
+      <c r="C16" s="7">
         <v>2.0</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="7">
         <v>1.0</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>42</v>
+      <c r="E16" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17">
-      <c r="C17" s="17">
+      <c r="C17" s="7">
         <v>3.0</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="7">
         <v>1.0</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>43</v>
+      <c r="E17" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18">
-      <c r="C18" s="17">
+      <c r="C18" s="7">
         <v>4.0</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="7">
         <v>1.0</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>44</v>
+      <c r="E18" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19">
-      <c r="C19" s="17">
+      <c r="C19" s="7">
         <v>5.0</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="7">
         <v>1.0</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>45</v>
+      <c r="E19" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="4"/>
     </row>
     <row r="20">
-      <c r="C20" s="17">
+      <c r="C20" s="7">
         <v>6.0</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="7">
         <v>1.0</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>46</v>
+      <c r="E20" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21">
-      <c r="C21" s="17">
+      <c r="C21" s="7">
         <v>7.0</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="7">
         <v>1.0</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>47</v>
+      <c r="E21" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22">
-      <c r="C22" s="17">
+      <c r="C22" s="7">
         <v>8.0</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="7">
         <v>1.0</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>48</v>
+      <c r="E22" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="4"/>
     </row>
     <row r="23">
-      <c r="C23" s="17">
+      <c r="C23" s="7">
         <v>9.0</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="7">
         <v>1.0</v>
       </c>
-      <c r="E23" s="18" t="s">
-        <v>49</v>
+      <c r="E23" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4"/>
     </row>
     <row r="24">
-      <c r="C24" s="17">
+      <c r="C24" s="7">
         <v>10.0</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="7">
         <v>1.0</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>50</v>
+      <c r="E24" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25">
-      <c r="C25" s="17">
+      <c r="C25" s="7">
         <v>11.0</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="7">
         <v>1.0</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>51</v>
+      <c r="E25" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="4"/>
     </row>
     <row r="26">
-      <c r="C26" s="17">
+      <c r="C26" s="7">
         <v>12.0</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="7">
         <v>1.0</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>52</v>
+      <c r="E26" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27">
-      <c r="C27" s="17">
+      <c r="C27" s="7">
         <v>13.0</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="7">
         <v>1.0</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>53</v>
+      <c r="E27" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28">
-      <c r="C28" s="17">
+      <c r="C28" s="7">
         <v>14.0</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="7">
         <v>1.0</v>
       </c>
-      <c r="E28" s="18" t="s">
-        <v>54</v>
+      <c r="E28" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="4"/>
     </row>
     <row r="29">
-      <c r="C29" s="17">
+      <c r="C29" s="7">
         <v>15.0</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>55</v>
+      <c r="D29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="4"/>
     </row>
     <row r="30">
-      <c r="C30" s="17">
+      <c r="C30" s="7">
         <v>16.0</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>56</v>
+      <c r="D30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -9326,7 +9287,7 @@
     </row>
     <row r="31">
       <c r="C31" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -9335,28 +9296,28 @@
       <c r="H31" s="4"/>
     </row>
     <row r="32">
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33">
-      <c r="C33" s="9">
+      <c r="C33" s="7">
         <v>1.0</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>58</v>
+      <c r="D33" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -9412,305 +9373,305 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.29"/>
-    <col customWidth="1" min="2" max="2" width="15.14"/>
-    <col customWidth="1" min="3" max="3" width="16.71"/>
-    <col customWidth="1" min="4" max="4" width="20.0"/>
-    <col customWidth="1" min="5" max="5" width="69.0"/>
-    <col customWidth="1" min="7" max="7" width="43.71"/>
-    <col customWidth="1" min="8" max="8" width="10.57"/>
-    <col customWidth="1" min="9" max="9" width="16.71"/>
+    <col customWidth="1" min="1" max="1" width="12.5"/>
+    <col customWidth="1" min="2" max="2" width="13.25"/>
+    <col customWidth="1" min="3" max="3" width="14.63"/>
+    <col customWidth="1" min="4" max="4" width="17.5"/>
+    <col customWidth="1" min="5" max="5" width="60.38"/>
+    <col customWidth="1" min="7" max="7" width="38.25"/>
+    <col customWidth="1" min="8" max="8" width="9.25"/>
+    <col customWidth="1" min="9" max="9" width="14.63"/>
   </cols>
   <sheetData>
     <row r="2">
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="26.25" customHeight="1">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="20" t="s">
+    </row>
+    <row r="6" ht="23.25" customHeight="1">
+      <c r="C6" s="5" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="C4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" ht="18.0" customHeight="1">
-      <c r="C6" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" ht="20.25" customHeight="1">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="13"/>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="9"/>
     </row>
     <row r="8">
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>1.0</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>1.0</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9">
-      <c r="C9" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="D9" s="9" t="s">
+    <row r="11">
+      <c r="C11" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="9" t="s">
+    </row>
+    <row r="12">
+      <c r="C12" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="C10" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="9" t="s">
+    </row>
+    <row r="13">
+      <c r="C13" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>40.0</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11">
-      <c r="C11" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="D11" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E11" s="9" t="s">
+    <row r="14">
+      <c r="C14" s="7">
+        <v>7.0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12">
-      <c r="C12" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="D12" s="9" t="s">
+    <row r="15">
+      <c r="C15" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="9" t="s">
+    </row>
+    <row r="16">
+      <c r="C16" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="D16" s="7">
+        <v>11.0</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13">
-      <c r="C13" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D13" s="9">
-        <v>40.0</v>
-      </c>
-      <c r="E13" s="9" t="s">
+    <row r="17">
+      <c r="C17" s="7">
+        <v>10.0</v>
+      </c>
+      <c r="D17" s="7">
+        <v>10.0</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14">
-      <c r="C14" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="D14" s="9">
+    <row r="18">
+      <c r="C18" s="7">
+        <v>11.0</v>
+      </c>
+      <c r="D18" s="7">
         <v>1.0</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E18" s="7" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" s="9">
-        <v>8.0</v>
-      </c>
-      <c r="D15" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="9">
-        <v>9.0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="C17" s="9">
-        <v>10.0</v>
-      </c>
-      <c r="D17" s="9">
-        <v>10.0</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="19" ht="22.5" customHeight="1">
       <c r="C19" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
-      <c r="G19" s="13"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" ht="19.5" customHeight="1">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>19</v>
+      <c r="E20" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="9">
+      <c r="C21" s="7">
         <v>1.0</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="7">
         <v>1.0</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22">
-      <c r="C22" s="9">
+    <row r="24">
+      <c r="C24" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="D26" s="7">
         <v>2.0</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="C23" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="9" t="s">
+      <c r="E26" s="7" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="C24" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="C25" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="D25" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="C26" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D26" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="27" ht="21.75" customHeight="1">
       <c r="C27" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" ht="21.75" customHeight="1">
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>19</v>
+      <c r="E28" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="9">
+      <c r="C29" s="7">
         <v>1.0</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>92</v>
+      <c r="D29" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>